<commit_message>
update dataset hotel feedback
</commit_message>
<xml_diff>
--- a/hotel.xlsx
+++ b/hotel.xlsx
@@ -318,11 +318,11 @@
       </c>
       <c r="B2" s="3">
         <f t="shared" ref="B2:B101" si="1">RANDBETWEEN(10,100)</f>
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4">
-        <f t="shared" ref="C2:C101" si="2">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <f t="shared" ref="C2:C101" si="2">RANDBETWEEN(1,10)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
@@ -331,11 +331,11 @@
       </c>
       <c r="B3" s="3">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
@@ -344,11 +344,11 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
@@ -357,11 +357,11 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -370,11 +370,11 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="1"/>
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="C6" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
@@ -383,11 +383,11 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -396,7 +396,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="2"/>
@@ -409,11 +409,11 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -422,11 +422,11 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
@@ -435,11 +435,11 @@
       </c>
       <c r="B11" s="3">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
@@ -448,7 +448,7 @@
       </c>
       <c r="B12" s="3">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C12" s="4">
         <f t="shared" si="2"/>
@@ -461,11 +461,11 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
@@ -474,11 +474,11 @@
       </c>
       <c r="B14" s="3">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C14" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -487,11 +487,11 @@
       </c>
       <c r="B15" s="3">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="C15" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
@@ -500,11 +500,11 @@
       </c>
       <c r="B16" s="3">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="C16" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
@@ -513,11 +513,11 @@
       </c>
       <c r="B17" s="3">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
@@ -526,11 +526,11 @@
       </c>
       <c r="B18" s="3">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C18" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
@@ -539,11 +539,11 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" si="1"/>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C19" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
@@ -552,11 +552,11 @@
       </c>
       <c r="B20" s="3">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C20" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -565,7 +565,7 @@
       </c>
       <c r="B21" s="3">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" si="2"/>
@@ -578,11 +578,11 @@
       </c>
       <c r="B22" s="3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -591,11 +591,11 @@
       </c>
       <c r="B23" s="3">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="C23" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -604,11 +604,11 @@
       </c>
       <c r="B24" s="3">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C24" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -617,11 +617,11 @@
       </c>
       <c r="B25" s="3">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -630,7 +630,7 @@
       </c>
       <c r="B26" s="3">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C26" s="4">
         <f t="shared" si="2"/>
@@ -643,11 +643,11 @@
       </c>
       <c r="B27" s="3">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -656,11 +656,11 @@
       </c>
       <c r="B28" s="3">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -669,11 +669,11 @@
       </c>
       <c r="B29" s="3">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -682,11 +682,11 @@
       </c>
       <c r="B30" s="3">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -695,11 +695,11 @@
       </c>
       <c r="B31" s="3">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -708,11 +708,11 @@
       </c>
       <c r="B32" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -721,11 +721,11 @@
       </c>
       <c r="B33" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="C33" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -734,11 +734,11 @@
       </c>
       <c r="B34" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C34" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -747,11 +747,11 @@
       </c>
       <c r="B35" s="3">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C35" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -760,11 +760,11 @@
       </c>
       <c r="B36" s="3">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C36" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -773,11 +773,11 @@
       </c>
       <c r="B37" s="3">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C37" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -786,11 +786,11 @@
       </c>
       <c r="B38" s="3">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -799,11 +799,11 @@
       </c>
       <c r="B39" s="3">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C39" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -812,11 +812,11 @@
       </c>
       <c r="B40" s="3">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C40" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -825,11 +825,11 @@
       </c>
       <c r="B41" s="3">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -838,11 +838,11 @@
       </c>
       <c r="B42" s="3">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="C42" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -851,11 +851,11 @@
       </c>
       <c r="B43" s="3">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C43" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -864,7 +864,7 @@
       </c>
       <c r="B44" s="3">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C44" s="4">
         <f t="shared" si="2"/>
@@ -877,11 +877,11 @@
       </c>
       <c r="B45" s="3">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C45" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -890,11 +890,11 @@
       </c>
       <c r="B46" s="3">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C46" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -903,11 +903,11 @@
       </c>
       <c r="B47" s="3">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C47" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -916,11 +916,11 @@
       </c>
       <c r="B48" s="3">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C48" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -929,11 +929,11 @@
       </c>
       <c r="B49" s="3">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C49" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
@@ -942,11 +942,11 @@
       </c>
       <c r="B50" s="3">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C50" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -955,11 +955,11 @@
       </c>
       <c r="B51" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C51" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -968,11 +968,11 @@
       </c>
       <c r="B52" s="3">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C52" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -981,11 +981,11 @@
       </c>
       <c r="B53" s="3">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -994,11 +994,11 @@
       </c>
       <c r="B54" s="3">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C54" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -1007,11 +1007,11 @@
       </c>
       <c r="B55" s="3">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="C55" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -1020,11 +1020,11 @@
       </c>
       <c r="B56" s="3">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C56" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -1033,11 +1033,11 @@
       </c>
       <c r="B57" s="3">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C57" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -1046,11 +1046,11 @@
       </c>
       <c r="B58" s="3">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C58" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
@@ -1059,11 +1059,11 @@
       </c>
       <c r="B59" s="3">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C59" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
@@ -1072,11 +1072,11 @@
       </c>
       <c r="B60" s="3">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C60" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -1085,11 +1085,11 @@
       </c>
       <c r="B61" s="3">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C61" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
@@ -1098,11 +1098,11 @@
       </c>
       <c r="B62" s="3">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="C62" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -1111,11 +1111,11 @@
       </c>
       <c r="B63" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C63" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="B64" s="3">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="C64" s="4">
         <f t="shared" si="2"/>
@@ -1137,11 +1137,11 @@
       </c>
       <c r="B65" s="3">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C65" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
@@ -1150,11 +1150,11 @@
       </c>
       <c r="B66" s="3">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C66" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
@@ -1163,11 +1163,11 @@
       </c>
       <c r="B67" s="3">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="C67" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -1176,11 +1176,11 @@
       </c>
       <c r="B68" s="3">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C68" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
@@ -1189,11 +1189,11 @@
       </c>
       <c r="B69" s="3">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="C69" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
@@ -1202,11 +1202,11 @@
       </c>
       <c r="B70" s="3">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="C70" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -1215,11 +1215,11 @@
       </c>
       <c r="B71" s="3">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C71" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B72" s="3">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C72" s="4">
         <f t="shared" si="2"/>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B73" s="3">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C73" s="4">
         <f t="shared" si="2"/>
@@ -1254,11 +1254,11 @@
       </c>
       <c r="B74" s="3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C74" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
@@ -1267,11 +1267,11 @@
       </c>
       <c r="B75" s="3">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C75" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
@@ -1280,11 +1280,11 @@
       </c>
       <c r="B76" s="3">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="C76" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
@@ -1293,11 +1293,11 @@
       </c>
       <c r="B77" s="3">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C77" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
@@ -1306,11 +1306,11 @@
       </c>
       <c r="B78" s="3">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C78" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="B79" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="C79" s="4">
         <f t="shared" si="2"/>
@@ -1332,11 +1332,11 @@
       </c>
       <c r="B80" s="3">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C80" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
@@ -1345,11 +1345,11 @@
       </c>
       <c r="B81" s="3">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="C81" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
@@ -1358,11 +1358,11 @@
       </c>
       <c r="B82" s="3">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C82" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
@@ -1371,11 +1371,11 @@
       </c>
       <c r="B83" s="3">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C83" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
@@ -1384,11 +1384,11 @@
       </c>
       <c r="B84" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C84" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B85" s="3">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C85" s="4">
         <f t="shared" si="2"/>
@@ -1410,11 +1410,11 @@
       </c>
       <c r="B86" s="3">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C86" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
@@ -1423,11 +1423,11 @@
       </c>
       <c r="B87" s="3">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C87" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B88" s="3">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="C88" s="4">
         <f t="shared" si="2"/>
@@ -1449,11 +1449,11 @@
       </c>
       <c r="B89" s="3">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C89" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
@@ -1462,11 +1462,11 @@
       </c>
       <c r="B90" s="3">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C90" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
@@ -1475,11 +1475,11 @@
       </c>
       <c r="B91" s="3">
         <f t="shared" si="1"/>
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C91" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="B92" s="3">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C92" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
@@ -1501,11 +1501,11 @@
       </c>
       <c r="B93" s="3">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C93" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
@@ -1514,11 +1514,11 @@
       </c>
       <c r="B94" s="3">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="C94" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
@@ -1527,11 +1527,11 @@
       </c>
       <c r="B95" s="3">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="C95" s="4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
@@ -1540,11 +1540,11 @@
       </c>
       <c r="B96" s="3">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C96" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B97" s="3">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C97" s="4">
         <f t="shared" si="2"/>
@@ -1566,11 +1566,11 @@
       </c>
       <c r="B98" s="3">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C98" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
@@ -1579,11 +1579,11 @@
       </c>
       <c r="B99" s="3">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="C99" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
@@ -1592,11 +1592,11 @@
       </c>
       <c r="B100" s="3">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="C100" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
@@ -1605,11 +1605,11 @@
       </c>
       <c r="B101" s="3">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="C101" s="4">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" ht="15.75" customHeight="1"/>

</xml_diff>